<commit_message>
+Added Negative Login Test Cases +Added XFail pytest marks
</commit_message>
<xml_diff>
--- a/Test_Cases.xlsx
+++ b/Test_Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OmarDorgham\OneDrive - ACT\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B7ECD6-B07E-458E-BE85-D8E3A97B63DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F194757-899D-4CD4-BD04-88762D87BBD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login - Positive" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="61">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -95,15 +95,6 @@
     <t>Click "Forgot password?" link and verify redirection</t>
   </si>
   <si>
-    <t>Try multiple invalid logins (brute-force)</t>
-  </si>
-  <si>
-    <t>Account should lock after a certain number of failed attempts</t>
-  </si>
-  <si>
-    <t>Attempt multiple failed login attempts consecutively</t>
-  </si>
-  <si>
     <t>Open login page in multiple browser tabs and attempt simultaneous logins</t>
   </si>
   <si>
@@ -128,15 +119,6 @@
     <t>username field is pre-filled or user remains logged in</t>
   </si>
   <si>
-    <t>Enter invalid username format (e.g., user@com, user.com)</t>
-  </si>
-  <si>
-    <t>Show "Invalid username format" error</t>
-  </si>
-  <si>
-    <t>Enter invalid username format and click Login</t>
-  </si>
-  <si>
     <t>Enter unregistered username and click Login</t>
   </si>
   <si>
@@ -195,12 +177,6 @@
   </si>
   <si>
     <t>TC-LOGIN-NEG-006</t>
-  </si>
-  <si>
-    <t>TC-LOGIN-NEG-007</t>
-  </si>
-  <si>
-    <t>TC-LOGIN-NEG-008</t>
   </si>
   <si>
     <t>TC-LOGIN-NEG-001</t>
@@ -316,16 +292,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="31">
     <dxf>
       <fill>
         <patternFill>
@@ -353,6 +320,15 @@
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -442,6 +418,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <top style="thin">
           <color auto="1"/>
@@ -505,7 +490,7 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="1" xr9:uid="{9EECE44B-5336-4CCF-982F-702DA4652318}">
-      <tableStyleElement type="wholeTable" dxfId="27"/>
+      <tableStyleElement type="wholeTable" dxfId="30"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -520,33 +505,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4DAD2762-7FDC-4566-AEF1-3A31EF287F56}" name="Table3" displayName="Table3" ref="A1:I7" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25" tableBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4DAD2762-7FDC-4566-AEF1-3A31EF287F56}" name="Table3" displayName="Table3" ref="A1:I7" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26">
   <autoFilter ref="A1:I7" xr:uid="{4DAD2762-7FDC-4566-AEF1-3A31EF287F56}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5A72C1FE-2764-4720-B6D8-C29C24F2D0D3}" name="Test Case ID" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{1FBF9763-493D-485F-9236-D0635F5CCDAD}" name="Scenario" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{A46C2532-02D9-4C32-B41A-5F1DBCF0FACC}" name="Expected Result" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{AB7DDC35-652B-40E3-842F-7A19D0D95C2F}" name="Test Steps" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{16AA09A8-6748-4F67-B9D9-956F63B2D15E}" name="Priority" dataDxfId="18"/>
-    <tableColumn id="6" xr3:uid="{457E8E6B-044E-4744-A6E1-B36A2C6D73A4}" name="Execution Status" dataDxfId="17"/>
-    <tableColumn id="7" xr3:uid="{F9011381-2906-4562-8561-C62E08A33F80}" name="Timestamp" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{72184A33-62C6-4978-8D27-289C0621550E}" name="Duration (s)" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{138A3D3C-533B-41FD-A1DB-F1D6E7240E31}" name="Actual Result" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{5A72C1FE-2764-4720-B6D8-C29C24F2D0D3}" name="Test Case ID" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{1FBF9763-493D-485F-9236-D0635F5CCDAD}" name="Scenario" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{A46C2532-02D9-4C32-B41A-5F1DBCF0FACC}" name="Expected Result" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{AB7DDC35-652B-40E3-842F-7A19D0D95C2F}" name="Test Steps" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{16AA09A8-6748-4F67-B9D9-956F63B2D15E}" name="Priority" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{457E8E6B-044E-4744-A6E1-B36A2C6D73A4}" name="Execution Status" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{F9011381-2906-4562-8561-C62E08A33F80}" name="Timestamp" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{72184A33-62C6-4978-8D27-289C0621550E}" name="Duration (s)" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{138A3D3C-533B-41FD-A1DB-F1D6E7240E31}" name="Actual Result" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DB51D7D4-71ED-44A6-97BF-744CD3BF4D87}" name="Table4" displayName="Table4" ref="A1:F9" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13">
-  <autoFilter ref="A1:F9" xr:uid="{DB51D7D4-71ED-44A6-97BF-744CD3BF4D87}"/>
-  <tableColumns count="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DB51D7D4-71ED-44A6-97BF-744CD3BF4D87}" name="Table4" displayName="Table4" ref="A1:I7" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13">
+  <autoFilter ref="A1:I7" xr:uid="{DB51D7D4-71ED-44A6-97BF-744CD3BF4D87}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{816B4DD9-83BF-4BFA-A32D-E79BD9C1BE15}" name="Test Case ID" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{D292F15E-D82B-48AB-8408-4E36D0B49367}" name="Scenario" dataDxfId="11"/>
     <tableColumn id="3" xr3:uid="{28C4620E-83B4-49AB-811B-824A6ACDFAEB}" name="Expected Result" dataDxfId="10"/>
     <tableColumn id="4" xr3:uid="{6F8509EB-43ED-45F0-BA56-48AB1440AD67}" name="Test Steps" dataDxfId="9"/>
     <tableColumn id="5" xr3:uid="{49CED559-6485-459F-AB30-8734FDB83B3C}" name="Priority" dataDxfId="8"/>
     <tableColumn id="6" xr3:uid="{586AE17C-C933-4487-A26E-BC9C25B60F46}" name="Execution Status" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{FA82997B-EED9-49A5-B079-BA20E2DE1914}" name="Timestamp" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{4AE66314-1F5C-4FCD-9FC6-23D23B0F938E}" name="Duration (s)" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{C9C79949-76C9-43D1-B66A-467CF8EA617F}" name="Actual Result" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -842,9 +830,9 @@
   </sheetPr>
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -880,21 +868,21 @@
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>6</v>
@@ -914,16 +902,16 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>8</v>
@@ -937,10 +925,10 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
@@ -960,13 +948,13 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>14</v>
@@ -983,7 +971,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>21</v>
@@ -1006,16 +994,16 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>20</v>
@@ -1030,10 +1018,10 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1049,11 +1037,11 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1064,10 +1052,13 @@
     <col min="4" max="4" width="52.1796875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="2"/>
+    <col min="7" max="7" width="14.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1086,59 +1077,68 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>8</v>
@@ -1147,18 +1147,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>8</v>
@@ -1167,18 +1167,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>8</v>
@@ -1187,18 +1187,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>8</v>
@@ -1207,52 +1207,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",F1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
++POSITIVE LOGOUT TCS ++ADDED SCREENSHOTS ON FAIL
</commit_message>
<xml_diff>
--- a/Test_Cases.xlsx
+++ b/Test_Cases.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OmarDorgham\OneDrive - ACT\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F194757-899D-4CD4-BD04-88762D87BBD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1C74A1-9402-4169-8584-CD0E0DAD2C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Login - Positive" sheetId="1" r:id="rId1"/>
-    <sheet name="Login - Negative" sheetId="2" r:id="rId2"/>
+    <sheet name="Authenticaion - Negative" sheetId="2" r:id="rId1"/>
+    <sheet name="Authentication - Positive" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="89">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -204,6 +204,90 @@
   </si>
   <si>
     <t>Actual Result</t>
+  </si>
+  <si>
+    <t>TC-LOGIN-NEG-007</t>
+  </si>
+  <si>
+    <t>TC-LOGIN-NEG-008</t>
+  </si>
+  <si>
+    <t>TC-LOGIN-POS-007</t>
+  </si>
+  <si>
+    <t>TC-LOGIN-POS-008</t>
+  </si>
+  <si>
+    <t>TC-LOGIN-POS-009</t>
+  </si>
+  <si>
+    <t>TC-LOGIN-POS-010</t>
+  </si>
+  <si>
+    <t>Verify successful logout from dashboard</t>
+  </si>
+  <si>
+    <t>User logs out successfully and redirects to login page</t>
+  </si>
+  <si>
+    <t>Login with valid credentials, click logout button, verify redirection</t>
+  </si>
+  <si>
+    <t>Verify logout from different pages within application</t>
+  </si>
+  <si>
+    <t>Logout works consistently from all authenticated pages</t>
+  </si>
+  <si>
+    <t>Navigate to various pages (dashboard, settings, profile), click logout from each</t>
+  </si>
+  <si>
+    <t>Verify browser back button after logout</t>
+  </si>
+  <si>
+    <t>Pressing back button after logout does not allow access to authenticated pages</t>
+  </si>
+  <si>
+    <t>Login, logout, press browser back button, verify redirect to login page</t>
+  </si>
+  <si>
+    <t>Verify direct URL access after logout</t>
+  </si>
+  <si>
+    <t>Cannot access protected pages via direct URL after logout</t>
+  </si>
+  <si>
+    <t>Logout, copy authenticated page URL, paste in browser, verify redirect to login</t>
+  </si>
+  <si>
+    <t>Verify re-login after logout with same credentials</t>
+  </si>
+  <si>
+    <t>User can immediately re-login with same credentials after logout</t>
+  </si>
+  <si>
+    <t>Login, logout, immediately login again with same credentials, verify success</t>
+  </si>
+  <si>
+    <t>Verify re-login after logout with different credentials</t>
+  </si>
+  <si>
+    <t>User can login with different account after logging out</t>
+  </si>
+  <si>
+    <t>Login with account A, logout, login with account B, verify successful switch</t>
+  </si>
+  <si>
+    <t>TC-LOGIN-POS-011</t>
+  </si>
+  <si>
+    <t>Verify logout button visibility after login</t>
+  </si>
+  <si>
+    <t>Logout button/option is visible only after successful login</t>
+  </si>
+  <si>
+    <t>Navigate to dashboard after login, verify logout button is present and clickable</t>
   </si>
 </sst>
 </file>
@@ -296,6 +380,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -303,7 +394,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -311,13 +402,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -505,36 +589,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4DAD2762-7FDC-4566-AEF1-3A31EF287F56}" name="Table3" displayName="Table3" ref="A1:I7" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26">
-  <autoFilter ref="A1:I7" xr:uid="{4DAD2762-7FDC-4566-AEF1-3A31EF287F56}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DB51D7D4-71ED-44A6-97BF-744CD3BF4D87}" name="Table4" displayName="Table4" ref="A1:I9" totalsRowShown="0" headerRowDxfId="29" dataDxfId="27" headerRowBorderDxfId="28" tableBorderDxfId="26">
+  <autoFilter ref="A1:I9" xr:uid="{DB51D7D4-71ED-44A6-97BF-744CD3BF4D87}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5A72C1FE-2764-4720-B6D8-C29C24F2D0D3}" name="Test Case ID" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{1FBF9763-493D-485F-9236-D0635F5CCDAD}" name="Scenario" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{A46C2532-02D9-4C32-B41A-5F1DBCF0FACC}" name="Expected Result" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{AB7DDC35-652B-40E3-842F-7A19D0D95C2F}" name="Test Steps" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{16AA09A8-6748-4F67-B9D9-956F63B2D15E}" name="Priority" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{457E8E6B-044E-4744-A6E1-B36A2C6D73A4}" name="Execution Status" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{F9011381-2906-4562-8561-C62E08A33F80}" name="Timestamp" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{72184A33-62C6-4978-8D27-289C0621550E}" name="Duration (s)" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{138A3D3C-533B-41FD-A1DB-F1D6E7240E31}" name="Actual Result" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{816B4DD9-83BF-4BFA-A32D-E79BD9C1BE15}" name="Test Case ID" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{D292F15E-D82B-48AB-8408-4E36D0B49367}" name="Scenario" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{28C4620E-83B4-49AB-811B-824A6ACDFAEB}" name="Expected Result" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{6F8509EB-43ED-45F0-BA56-48AB1440AD67}" name="Test Steps" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{49CED559-6485-459F-AB30-8734FDB83B3C}" name="Priority" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{586AE17C-C933-4487-A26E-BC9C25B60F46}" name="Execution Status" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{FA82997B-EED9-49A5-B079-BA20E2DE1914}" name="Timestamp" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{4AE66314-1F5C-4FCD-9FC6-23D23B0F938E}" name="Duration (s)" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{C9C79949-76C9-43D1-B66A-467CF8EA617F}" name="Actual Result" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{DB51D7D4-71ED-44A6-97BF-744CD3BF4D87}" name="Table4" displayName="Table4" ref="A1:I7" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13">
-  <autoFilter ref="A1:I7" xr:uid="{DB51D7D4-71ED-44A6-97BF-744CD3BF4D87}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4DAD2762-7FDC-4566-AEF1-3A31EF287F56}" name="Table3" displayName="Table3" ref="A1:I12" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13">
+  <autoFilter ref="A1:I12" xr:uid="{4DAD2762-7FDC-4566-AEF1-3A31EF287F56}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{816B4DD9-83BF-4BFA-A32D-E79BD9C1BE15}" name="Test Case ID" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{D292F15E-D82B-48AB-8408-4E36D0B49367}" name="Scenario" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{28C4620E-83B4-49AB-811B-824A6ACDFAEB}" name="Expected Result" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{6F8509EB-43ED-45F0-BA56-48AB1440AD67}" name="Test Steps" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{49CED559-6485-459F-AB30-8734FDB83B3C}" name="Priority" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{586AE17C-C933-4487-A26E-BC9C25B60F46}" name="Execution Status" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{FA82997B-EED9-49A5-B079-BA20E2DE1914}" name="Timestamp" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{4AE66314-1F5C-4FCD-9FC6-23D23B0F938E}" name="Duration (s)" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{C9C79949-76C9-43D1-B66A-467CF8EA617F}" name="Actual Result" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{5A72C1FE-2764-4720-B6D8-C29C24F2D0D3}" name="Test Case ID" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{1FBF9763-493D-485F-9236-D0635F5CCDAD}" name="Scenario" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{A46C2532-02D9-4C32-B41A-5F1DBCF0FACC}" name="Expected Result" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{AB7DDC35-652B-40E3-842F-7A19D0D95C2F}" name="Test Steps" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{16AA09A8-6748-4F67-B9D9-956F63B2D15E}" name="Priority" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{457E8E6B-044E-4744-A6E1-B36A2C6D73A4}" name="Execution Status" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{F9011381-2906-4562-8561-C62E08A33F80}" name="Timestamp" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{72184A33-62C6-4978-8D27-289C0621550E}" name="Duration (s)" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{138A3D3C-533B-41FD-A1DB-F1D6E7240E31}" name="Actual Result" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -824,232 +908,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <tabColor rgb="FF00B050"/>
-  </sheetPr>
-  <dimension ref="A1:I7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="62.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.26953125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Failed">
-      <formula>NOT(ISERROR(SEARCH("Failed",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Passed">
-      <formula>NOT(ISERROR(SEARCH("Passed",F1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08239121-B1A4-44B2-B9BA-C46924203ECB}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.7265625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.54296875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.54296875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.36328125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.7265625" style="2" bestFit="1" customWidth="1"/>
@@ -1207,13 +1082,53 @@
         <v>9</v>
       </c>
     </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="F1:F1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Passed">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Passed">
       <formula>NOT(ISERROR(SEARCH("Passed",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Failed">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Failed">
       <formula>NOT(ISERROR(SEARCH("Failed",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1222,4 +1137,329 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="F1:F1048576">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Failed">
+      <formula>NOT(ISERROR(SEARCH("Failed",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Passed">
+      <formula>NOT(ISERROR(SEARCH("Passed",F1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>